<commit_message>
Allow user to change port of dash app
</commit_message>
<xml_diff>
--- a/template_case.xlsx
+++ b/template_case.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">asset</t>
   </si>
@@ -81,7 +81,7 @@
     <t xml:space="preserve">case</t>
   </si>
   <si>
-    <t xml:space="preserve">D</t>
+    <t xml:space="preserve">BPV</t>
   </si>
   <si>
     <t xml:space="preserve">D for diesel genset only; BPV for battery and PV; DBPV for battery PV and diesel genset (only those 3 cases are covered for now)</t>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t xml:space="preserve">Maximal percentage by which the non critical demand (“Demand” column of the “timeseries” sheet) is allowed to be reduced in one timestep, if demand is 100 and maximum_demand_reduction 0.25, then the demand supplied can span between 75 and 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port number on which the dash app displays</t>
   </si>
 </sst>
 </file>
@@ -106,6 +112,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -197,7 +204,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -261,9 +268,9 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.07"/>
   </cols>
@@ -282,7 +289,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -295,13 +302,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -358,10 +365,21 @@
         <v>22</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>8050</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add parser to sensitivity inputs
</commit_message>
<xml_diff>
--- a/template_case.xlsx
+++ b/template_case.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="costs" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="timeseries" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="settings" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="sensitivity" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t xml:space="preserve">asset</t>
   </si>
@@ -160,6 +161,27 @@
   </si>
   <si>
     <t xml:space="preserve">This is also known sometimes as discount factor or discount rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">variable_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min_val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">step</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should either “settings” or one of the assets of the tab “costs”, for example battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the variable you would like to vary</t>
   </si>
 </sst>
 </file>
@@ -263,8 +285,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="A1:E2 B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -389,7 +411,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8739" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -429,7 +451,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="A1:E2 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -509,6 +531,55 @@
       </c>
       <c r="C7" s="0" t="s">
         <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add possibility to change the min and max soc level
</commit_message>
<xml_diff>
--- a/template_case.xlsx
+++ b/template_case.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="costs" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">asset</t>
   </si>
@@ -161,6 +161,18 @@
   </si>
   <si>
     <t xml:space="preserve">This is also known sometimes as discount factor or discount rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_soc_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule for lower bound constraint for the storage content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">storage_soc_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule for upper bound constraint for the storage content</t>
   </si>
   <si>
     <t xml:space="preserve">category</t>
@@ -286,10 +298,10 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="1" sqref="A1:E2 B12"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
@@ -411,10 +423,10 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8739" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A1:E2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.91"/>
@@ -448,13 +460,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="A1:E2 B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -531,6 +543,28 @@
       </c>
       <c r="C7" s="0" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -551,35 +585,35 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>